<commit_message>
v0.3.0 - Month summary complete. Db extended for targets of Day0
</commit_message>
<xml_diff>
--- a/temp_data/import_me.xlsx
+++ b/temp_data/import_me.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plr03474\NoOneDrive\Python\myMonth\mymonth\static\initial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{955B4222-633F-45F4-88A2-60BFBC22F857}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23ACC805-5301-4124-8AA5-B1A6E21567EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="days" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -131,6 +131,18 @@
     <t>3h 46m</t>
   </si>
   <si>
+    <t>10m</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>2h 49m</t>
+  </si>
+  <si>
+    <t>days0</t>
+  </si>
+  <si>
     <t>10h</t>
   </si>
   <si>
@@ -138,9 +150,6 @@
   </si>
   <si>
     <t>15h</t>
-  </si>
-  <si>
-    <t>20h</t>
   </si>
 </sst>
 </file>
@@ -150,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,22 +172,6 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -188,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -211,42 +204,19 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{7187AEC6-6560-4D8A-8C12-598D9DE8092C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -546,11 +516,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,8 +818,66 @@
       <c r="C21" t="s">
         <v>35</v>
       </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
       <c r="H21">
         <v>3.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44248</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44249</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>44250</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>44251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>44252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>44253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>44254</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>44255</v>
       </c>
     </row>
   </sheetData>
@@ -858,11 +886,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAA221C-D12A-4900-B428-82C3D6FDDEA4}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,71 +899,59 @@
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>44228</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="6">
+      <c r="H2">
         <v>3.12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
-        <v>44256</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="6">
-        <v>2.86</v>
+      <c r="I2">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v0.5.0 Historical data for aggegated months now importable from excel
</commit_message>
<xml_diff>
--- a/temp_data/import_me.xlsx
+++ b/temp_data/import_me.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\plr03474\NoOneDrive\Python\myMonth\mymonth\static\initial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23ACC805-5301-4124-8AA5-B1A6E21567EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6715834C-0752-4029-BB8C-FDA2D4DA4AEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="days" sheetId="1" r:id="rId1"/>
     <sheet name="monthly_targets" sheetId="2" r:id="rId2"/>
+    <sheet name="historical_scores" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -150,6 +151,111 @@
   </si>
   <si>
     <t>15h</t>
+  </si>
+  <si>
+    <t>18m07</t>
+  </si>
+  <si>
+    <t>18m08</t>
+  </si>
+  <si>
+    <t>18m09</t>
+  </si>
+  <si>
+    <t>18m10</t>
+  </si>
+  <si>
+    <t>18m11</t>
+  </si>
+  <si>
+    <t>18m12</t>
+  </si>
+  <si>
+    <t>19m01</t>
+  </si>
+  <si>
+    <t>19m02</t>
+  </si>
+  <si>
+    <t>19m03</t>
+  </si>
+  <si>
+    <t>19m04</t>
+  </si>
+  <si>
+    <t>19m05</t>
+  </si>
+  <si>
+    <t>19m06</t>
+  </si>
+  <si>
+    <t>19m07</t>
+  </si>
+  <si>
+    <t>19m08</t>
+  </si>
+  <si>
+    <t>19m09</t>
+  </si>
+  <si>
+    <t>19m10</t>
+  </si>
+  <si>
+    <t>19m11</t>
+  </si>
+  <si>
+    <t>19m12</t>
+  </si>
+  <si>
+    <t>20m01</t>
+  </si>
+  <si>
+    <t>20m02</t>
+  </si>
+  <si>
+    <t>20m03</t>
+  </si>
+  <si>
+    <t>20m04</t>
+  </si>
+  <si>
+    <t>20m05</t>
+  </si>
+  <si>
+    <t>20m06</t>
+  </si>
+  <si>
+    <t>20m07</t>
+  </si>
+  <si>
+    <t>20m08</t>
+  </si>
+  <si>
+    <t>20m09</t>
+  </si>
+  <si>
+    <t>20m10</t>
+  </si>
+  <si>
+    <t>20m11</t>
+  </si>
+  <si>
+    <t>20m12</t>
+  </si>
+  <si>
+    <t>21m01</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>day0</t>
+  </si>
+  <si>
+    <t>ml</t>
   </si>
 </sst>
 </file>
@@ -157,7 +263,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -208,12 +314,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,8 +626,8 @@
   <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,9 +996,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,4 +1061,468 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2948D19B-DEDC-49F9-A77C-4564A4A3BC2A}">
+  <dimension ref="A1:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.47670000000000001</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.14219999999999999</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.46589999999999998</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.44540000000000002</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.48060000000000003</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.3931</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.8286</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.874</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.65069999999999995</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.1186</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.121</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.82489999999999997</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.63700000000000001</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.71550000000000002</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.0149999999999999</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.86719999999999997</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.93520000000000003</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="3">
+        <v>0.63560000000000005</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.91849999999999998</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.72309999999999997</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1.2712000000000001</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1.0843</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="3">
+        <v>0.63070000000000004</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1.1800999999999999</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1.0217000000000001</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="3">
+        <v>0.63229999999999997</v>
+      </c>
+      <c r="C27">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="3">
+        <v>0.24709999999999999</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="3">
+        <v>0.52429999999999999</v>
+      </c>
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="3">
+        <v>0.76559999999999995</v>
+      </c>
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" s="3">
+        <v>0.45789999999999997</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1.0492999999999999</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>421</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>